<commit_message>
fix lots of things... loadings in R script, python script can now read comma separated strings as lists correctly
</commit_message>
<xml_diff>
--- a/trait_processing/Trait_term_reconciliation.xlsx
+++ b/trait_processing/Trait_term_reconciliation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanfolk/Documents/GitHub/fagales_traits/trait_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDD65D3-D985-494E-BB47-6D8BE0FE40CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D07BE26-FFB0-E147-BD61-124751112D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="500" windowWidth="24960" windowHeight="14740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15460" yWindow="500" windowWidth="24960" windowHeight="14740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infl  Trait-WHOLE-term synonyms" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="163">
   <si>
     <t>corymbose cymes</t>
   </si>
@@ -500,6 +500,36 @@
   </si>
   <si>
     <t>villous</t>
+  </si>
+  <si>
+    <t>doubly toothed</t>
+  </si>
+  <si>
+    <t>doubly-toothed</t>
+  </si>
+  <si>
+    <t>double-toothed</t>
+  </si>
+  <si>
+    <t>subacuminate</t>
+  </si>
+  <si>
+    <t>acuminate</t>
+  </si>
+  <si>
+    <t>sub-acuminate</t>
+  </si>
+  <si>
+    <t>coarsely toothed</t>
+  </si>
+  <si>
+    <t>dentate</t>
+  </si>
+  <si>
+    <t>finely toothed</t>
+  </si>
+  <si>
+    <t>serrate</t>
   </si>
 </sst>
 </file>
@@ -1150,15 +1180,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1599,6 +1630,54 @@
       </c>
       <c r="B55" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>158</v>
+      </c>
+      <c r="B59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>161</v>
+      </c>
+      <c r="B61" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>